<commit_message>
New version of effectivity comparison
</commit_message>
<xml_diff>
--- a/Efficiency_comparison.xlsx
+++ b/Efficiency_comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>My program</t>
+          <t>Sizes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>My project</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>enumerative_backtracking_solver.py</t>
         </is>
       </c>
     </row>
@@ -451,8 +461,16 @@
           <t>test70419.txt</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>2.261542081832886</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>21*25</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3.737349033355713</v>
+      </c>
+      <c r="D2" t="n">
+        <v>64.78196930885315</v>
       </c>
     </row>
     <row r="3">
@@ -461,8 +479,16 @@
           <t>test70402.txt</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.3399569988250732</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>24*18</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1.997181177139282</v>
+      </c>
+      <c r="D3" t="n">
+        <v>21.54502701759338</v>
       </c>
     </row>
     <row r="4">
@@ -471,128 +497,70 @@
           <t>test70399.txt</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.1861388683319092</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>18*29</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1.694288015365601</v>
+      </c>
+      <c r="D4" t="n">
+        <v>336.943610906601</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test70472.txt</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.3348798751831055</v>
+          <t>test70446.txt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22*45</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2.374522924423218</v>
+      </c>
+      <c r="D5" t="n">
+        <v>141.6387090682983</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test70449.txt</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.1728911399841309</v>
+          <t>test70470.txt</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>45*41</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4.309165954589844</v>
+      </c>
+      <c r="D6" t="n">
+        <v>468.6386382579803</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>test70446.txt</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.3276352882385254</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>test70474.txt</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.3379311561584473</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>test70470.txt</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.3343019485473633</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
           <t>test70468.txt</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>0.3195099830627441</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>test70442.txt</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.236781120300293</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>test70281.txt</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.4800410270690918</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>test70260.txt</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.2084639072418213</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>test70289.txt</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.5151848793029785</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>test70070.txt</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.5896039009094238</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>test69690.txt</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.5377321243286133</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>45*45</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6.089066982269287</v>
+      </c>
+      <c r="D7" t="n">
+        <v>321.1132562160492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unsat tests results added
</commit_message>
<xml_diff>
--- a/Efficiency_comparison.xlsx
+++ b/Efficiency_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariafadeeva/PycharmProjects/Nonogram-solver-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19461A0-4390-3243-8A33-E4D2930FABCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EA5EAE-3AA7-5045-8800-DCD5DA2581BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>New_solver.py</t>
   </si>
@@ -215,6 +215,42 @@
   </si>
   <si>
     <t>46.74534607</t>
+  </si>
+  <si>
+    <t>unsat_test_1.txt</t>
+  </si>
+  <si>
+    <t>unsat_test_2.txt</t>
+  </si>
+  <si>
+    <t>unsat_test_3.txt</t>
+  </si>
+  <si>
+    <t>10*11</t>
+  </si>
+  <si>
+    <t>11*11</t>
+  </si>
+  <si>
+    <t>31*15</t>
+  </si>
+  <si>
+    <t>87.87386393547058</t>
+  </si>
+  <si>
+    <t>112.05067491531372</t>
+  </si>
+  <si>
+    <t>0.04214024543762207</t>
+  </si>
+  <si>
+    <t>0.03474092483520508</t>
+  </si>
+  <si>
+    <t>0.03778791427612305</t>
+  </si>
+  <si>
+    <t>0.2221817970275879</t>
   </si>
 </sst>
 </file>
@@ -236,13 +272,6 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="14"/>
-      <color rgb="FF1155CC"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF212121"/>
       <name val="Courier New"/>
@@ -255,6 +284,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -276,14 +311,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -587,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,10 +647,10 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -626,7 +661,7 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -643,7 +678,7 @@
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -660,7 +695,7 @@
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -674,10 +709,10 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -691,10 +726,10 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -711,7 +746,7 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -725,10 +760,10 @@
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -745,7 +780,7 @@
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -762,7 +797,7 @@
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -776,10 +811,10 @@
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -793,10 +828,10 @@
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -810,10 +845,10 @@
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -827,10 +862,10 @@
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -844,10 +879,10 @@
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -861,16 +896,67 @@
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>